<commit_message>
Them CSDL VLXD.bak va Tao Test Case Dang nhap
</commit_message>
<xml_diff>
--- a/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
+++ b/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>1.    Phạm vi test</t>
   </si>
@@ -125,17 +125,144 @@
     <t>Nguyễn Ngọc Huy</t>
   </si>
   <si>
-    <t>TC-001</t>
-  </si>
-  <si>
     <t>Test Case For Store Construction Materials Management</t>
+  </si>
+  <si>
+    <t>SCM-001</t>
+  </si>
+  <si>
+    <t>SCM-003</t>
+  </si>
+  <si>
+    <t>SCM-004</t>
+  </si>
+  <si>
+    <t>SCM-005</t>
+  </si>
+  <si>
+    <t>Đăng nhập</t>
+  </si>
+  <si>
+    <t>Đã có tên đăng nhập và mật khẩu</t>
+  </si>
+  <si>
+    <t>- Đăng nhập thành công
+- Hiển thị Form "Đặt hàng".</t>
+  </si>
+  <si>
+    <t>Đăng nhập hệ thống 
+(Bấm nút Đăng nhập)</t>
+  </si>
+  <si>
+    <t>SCM-002</t>
+  </si>
+  <si>
+    <t>Đăng nhập hệ thống 
+(Nhấn phím Enter)</t>
+  </si>
+  <si>
+    <t>1. Điền tên đăng nhập: Huy
+2. Điền mật khẩu: 123
+3. Nhấn phím Enter</t>
+  </si>
+  <si>
+    <t>1. Điền tên đăng nhập: Huy
+2. Điền mật khẩu: 123
+3. Bấm nút "Đăng nhập".</t>
+  </si>
+  <si>
+    <t>Đăng nhập hệ thống 
+(Điền tên đăng nhập 
+- bỏ trống Mật khẩu)</t>
+  </si>
+  <si>
+    <t>Đã có tên đăng nhập, không có mật khẩu</t>
+  </si>
+  <si>
+    <t>1. Điền tên đăng nhập: Huy
+2. Bấm nút "Đăng nhập"</t>
+  </si>
+  <si>
+    <t>- Hiển thị hộp thoại thông báo "Bạn phải nhập mật khẩu".
+- Không thể vào hệ thống, quay lại Form "Đăng nhập".</t>
+  </si>
+  <si>
+    <t>Đăng nhập hệ thống 
+(Nhập sai tên đăng nhập - Nhập sai mật khẩu)</t>
+  </si>
+  <si>
+    <t>Không có tên đăng nhập và mật khẩu</t>
+  </si>
+  <si>
+    <t>1. Điền tên đăng nhập: abc
+2. Điền mật khẩu: abc456
+3. Bấm nút "Đăng nhập".</t>
+  </si>
+  <si>
+    <t>- Hiển thị hộp thoại thông báo "Bạn đã nhập sai tên đăng nhập và mật khẩu - Yêu cầu đăng nhập lại".
+- Không thể vào hệ thống, quay lại Form "Đăng nhập".</t>
+  </si>
+  <si>
+    <t>Đăng nhập hệ thống 
+(Nhập đúng tên đăng nhập - Nhập sai mật khẩu)</t>
+  </si>
+  <si>
+    <t>Có tên đăng nhập và không có mật khẩu</t>
+  </si>
+  <si>
+    <t>1. Điền tên đăng nhập: Huy
+2. Điền mật khẩu: 456
+3. Bấm nút "Đăng nhập".</t>
+  </si>
+  <si>
+    <t>- Hiển thị hộp thoại thông báo "Bạn đã nhập sai mật khẩu" - Yêu cầu đăng nhập lại.
+- Không thể vào hệ thống, quay lại Form "Đăng nhập".</t>
+  </si>
+  <si>
+    <t>Đăng nhập hệ thống 
+(Kiểm tra nút ẩn - hiển mật khẩu)</t>
+  </si>
+  <si>
+    <t>Phải có nhập mật khẩu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Điền mật khẩu: 123
+2. Bấm nút  </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Mật khẩu chuyển từ dạng " </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>···</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> " sang " 123 " và ngược lại nếu nhấn nút          lần nữa.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>SCM-006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +331,13 @@
     </font>
     <font>
       <sz val="24"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -630,50 +764,50 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1278,6 +1412,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>992028</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>326222</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7067550" y="4933950"/>
+          <a:ext cx="258603" cy="145247"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1381125</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1639728</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>411947</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9715500" y="5019675"/>
+          <a:ext cx="258603" cy="145247"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1601,7 +1828,7 @@
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
+      <c r="E1" s="59"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -1610,47 +1837,47 @@
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="54" t="s">
+      <c r="I2" s="52"/>
+      <c r="J2" s="53" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="55"/>
+      <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
@@ -1701,7 +1928,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="44"/>
-      <c r="C7" s="48"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="17"/>
       <c r="E7" s="13"/>
       <c r="F7" s="5"/>
@@ -1716,8 +1943,8 @@
       <c r="C8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="15"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1730,8 +1957,8 @@
       <c r="C9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="15"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -1744,8 +1971,8 @@
       <c r="C10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
       <c r="F10" s="15"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1777,11 +2004,11 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -1804,6 +2031,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="G2:G3"/>
@@ -1813,11 +2045,6 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1828,8 +2055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1850,7 +2077,7 @@
   <sheetData>
     <row r="1" spans="1:22" s="30" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -1907,15 +2134,27 @@
         <v>1</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="22"/>
+        <v>32</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="23">
+        <v>1</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="28"/>
+      <c r="H3" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="J3" s="20"/>
       <c r="K3" s="24"/>
       <c r="L3" s="19"/>
@@ -1925,14 +2164,28 @@
       <c r="A4" s="24">
         <v>2</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="22"/>
+      <c r="B4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="23">
+        <v>1</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="28"/>
+      <c r="H4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="J4" s="20"/>
       <c r="K4" s="24"/>
       <c r="L4" s="19"/>
@@ -1941,14 +2194,28 @@
       <c r="A5" s="24">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="22"/>
+      <c r="B5" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="28"/>
+      <c r="H5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>47</v>
+      </c>
       <c r="J5" s="20"/>
       <c r="K5" s="24"/>
       <c r="L5" s="19"/>
@@ -1957,14 +2224,28 @@
       <c r="A6" s="24">
         <v>4</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="22"/>
+      <c r="B6" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="23">
+        <v>1</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="28"/>
+      <c r="H6" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>51</v>
+      </c>
       <c r="J6" s="20"/>
       <c r="K6" s="24"/>
       <c r="L6" s="19"/>
@@ -1973,14 +2254,28 @@
       <c r="A7" s="24">
         <v>5</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="22"/>
+      <c r="B7" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="23">
+        <v>1</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>53</v>
+      </c>
       <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="28"/>
+      <c r="H7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>55</v>
+      </c>
       <c r="J7" s="20"/>
       <c r="K7" s="24"/>
       <c r="L7" s="19"/>
@@ -1989,14 +2284,28 @@
       <c r="A8" s="24">
         <v>6</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
+      <c r="B8" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="23">
+        <v>1</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>59</v>
+      </c>
       <c r="J8" s="19"/>
       <c r="K8" s="24"/>
       <c r="L8" s="19"/>
@@ -3582,6 +3891,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Test Case Khach hang - Huy
</commit_message>
<xml_diff>
--- a/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
+++ b/TestCase_QuanLyCuaHangVatLieuXayDung.xlsx
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DB_Test_case!$A$2:$I$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Case'!$A$2:$L$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Case'!$A$2:$L$89</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="116">
   <si>
     <t>1.    Phạm vi test</t>
   </si>
@@ -256,6 +256,229 @@
   </si>
   <si>
     <t>SCM-006</t>
+  </si>
+  <si>
+    <t>Khách hàng</t>
+  </si>
+  <si>
+    <t>Xem thông tin khách hàng</t>
+  </si>
+  <si>
+    <t>Đã đăng nhập thành công</t>
+  </si>
+  <si>
+    <t>Đăng nhập hệ thống</t>
+  </si>
+  <si>
+    <t>1. Nhấn vào hàng hoặc cột bất kỳ của bảng khách hàng.
+2. Xem thông tin được hiển thị phía trên theo từng trường dữ liệu</t>
+  </si>
+  <si>
+    <t>- Hiển thị đúng thông tin của hàng/cột dữ liệu được chọn lên trên textbox phía trên.</t>
+  </si>
+  <si>
+    <t>SCM-007</t>
+  </si>
+  <si>
+    <t>SCM-009</t>
+  </si>
+  <si>
+    <t>SCM-008</t>
+  </si>
+  <si>
+    <t>Thêm khách hàng mới (Không cho phép nhập Mã khách hàng)</t>
+  </si>
+  <si>
+    <t>Thêm khách hàng mới (Không nhập dữ liệu cho khách hàng mới được thêm)</t>
+  </si>
+  <si>
+    <t>1. Nhập đầy đủ thông tin khách hàng: Họ, tên, địa chỉ, số điện thoại, giới tính
+2. Bấm nút "Thêm".</t>
+  </si>
+  <si>
+    <t>1. Để trống tất cả các hộp: Họ, tên, địa chỉ, số điện thoại.
+2. Bấm nút "Thêm".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hiển thị thông báo "Bạn phải nhập thông tin cho khách hàng cần thêm".
+- Không thể thêm mới khách hàng. </t>
+  </si>
+  <si>
+    <t>SCM-010</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo "Khách hàng được thêm mới thành công" và hiển thị trong danh sách khách hàng.
+- Mã khách hàng tự động sinh ra trong CSDL.</t>
+  </si>
+  <si>
+    <t>Thêm khách hàng mới (Nhập không đầy đủ thông tin khách hàng)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Hiển thị thông báo "Bạn phải nhập </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đầy đủ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> thông tin cho khách hàng cần thêm".
+- Không thể thêm mới khách hàng. </t>
+    </r>
+  </si>
+  <si>
+    <t>SCM-011</t>
+  </si>
+  <si>
+    <t>SCM-013</t>
+  </si>
+  <si>
+    <t>SCM-014</t>
+  </si>
+  <si>
+    <t>1. Nhập dữ liệu và để trống một trong số các hộp: Họ, tên, địa chỉ, số điện thoại.
+2. Bấm nút "Thêm".</t>
+  </si>
+  <si>
+    <t>1. Nhấn vào hàng hoặc cột bất kỳ của bảng khách hàng.
+2. Sửa lại thông tin trên các textbox thông tin
+3. Bấm nút "Sửa"</t>
+  </si>
+  <si>
+    <t>Sửa thông tin khách hàng (Không cho phép sửa mã khách hàng)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Thông tin mã khách hàng Disable.
+- Hiển thị thông báo "Khách hàng được sửa thành công" và hiển thị lại thông tin được sửa trong danh sách khách hàng.
+</t>
+  </si>
+  <si>
+    <t>SCM-012</t>
+  </si>
+  <si>
+    <t>Sửa thông tin khách hàng (Xóa các thông tin được hiển thị trên textbox)</t>
+  </si>
+  <si>
+    <t>1. Nhấn vào hàng hoặc cột bất kỳ của bảng khách hàng.
+2. Xóa hết tất cả thông tin được hiển thị trên textbox
+3. Bấm nút "Sửa"</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo "Không được sửa nếu như thiếu thông tin khách hàng".
+- Sửa thông tin khách hàng thất bại.</t>
+  </si>
+  <si>
+    <t>SCM-015</t>
+  </si>
+  <si>
+    <t>SCM-016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm kiếm khách hàng theo tên
+(Nhập đúng tên có dấu) </t>
+  </si>
+  <si>
+    <t>1. Tick chọn "Theo tên".
+2. Điền vào ô tìm kiếm: Dung
+3. Bấm nút "Tìm".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm kiếm khách hàng theo tên
+(Nhập tên định dạng thường và không dấu) </t>
+  </si>
+  <si>
+    <t>1. Tick chọn "Theo tên".
+2. Điền vào ô tìm kiếm: hong
+3. Bấm nút "Tìm".</t>
+  </si>
+  <si>
+    <t>- Hiển thị một hoặc một danh sách các hàng dữ liệu có liên quan đến tên được nhập.</t>
+  </si>
+  <si>
+    <t>- Hiển thị hàng dữ liệu khách hàng được tìm kiếm theo tên được nhập.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm kiếm khách hàng theo tên
+(Tìm khách hàng không tên có trong danh sách Khách hàng) </t>
+  </si>
+  <si>
+    <t>1. Tick chọn "Theo tên".
+2. Điền vào ô tìm kiếm: Yến
+3. Bấm nút "Tìm".</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo "Không có khách hàng theo tên được tìm kiếm"
+- Tìm kiếm thất bại.</t>
+  </si>
+  <si>
+    <t>Tìm kiếm khách hàng theo mã khách hàng
+(Nhập đúng mã khách hàng)</t>
+  </si>
+  <si>
+    <t>- Hiển thị hàng dữ liệu khách hàng được tìm kiếm theo mã khách hàng được nhập.</t>
+  </si>
+  <si>
+    <t>1. Tick chọn "Theo mã".
+2. Điền vào ô tìm kiếm: 3
+3. Bấm nút "Tìm".</t>
+  </si>
+  <si>
+    <t>SCM-017</t>
+  </si>
+  <si>
+    <t>1. Tick chọn "Theo mã".
+2. Điền vào ô tìm kiếm: 100
+3. Bấm nút "Tìm".</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo "Không có khách hàng theo mã được tìm kiếm"
+- Tìm kiếm thất bại.</t>
+  </si>
+  <si>
+    <t>SCM-018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm kiếm khách hàng theo tên
+(Để trống ô tìm kiếm) </t>
+  </si>
+  <si>
+    <t>1. Tick chọn "Theo tên".
+2. Bấm nút "Tìm".</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo "Bạn phải nhập tên khách hàng cần tìm kiếm"
+- Tìm kiếm thất bại.</t>
+  </si>
+  <si>
+    <t>SCM-019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm kiếm khách hàng theo mã 
+(Để trống ô tìm kiếm) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm kiếm khách hàng theo mã khách hàng
+(Tìm khách hàng không mã có trong danh sách Khách hàng) </t>
+  </si>
+  <si>
+    <t>1. Tick chọn "Theo mã".
+2. Bấm nút "Tìm".</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo "Bạn phải nhập mã khách hàng cần tìm kiếm"
+- Tìm kiếm thất bại.</t>
   </si>
 </sst>
 </file>
@@ -764,6 +987,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -776,12 +1008,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -805,9 +1031,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -819,7 +1042,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="83">
+  <dxfs count="89">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1828,7 +2093,7 @@
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
-      <c r="E1" s="59"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -1837,47 +2102,47 @@
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="I2" s="53"/>
+      <c r="J2" s="54" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="54"/>
+      <c r="J3" s="55"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
@@ -1928,7 +2193,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="17"/>
       <c r="E7" s="13"/>
       <c r="F7" s="5"/>
@@ -1943,8 +2208,8 @@
       <c r="C8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="15"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1957,8 +2222,8 @@
       <c r="C9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="15"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -1971,8 +2236,8 @@
       <c r="C10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="59"/>
       <c r="F10" s="15"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -2004,11 +2269,11 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -2031,11 +2296,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="G2:G3"/>
@@ -2045,6 +2305,11 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -2053,10 +2318,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V88"/>
+  <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2314,14 +2579,30 @@
       <c r="A9" s="24">
         <v>7</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="B9" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="23">
+        <v>2</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>66</v>
+      </c>
       <c r="J9" s="19"/>
       <c r="K9" s="24"/>
       <c r="L9" s="19"/>
@@ -2330,14 +2611,30 @@
       <c r="A10" s="24">
         <v>8</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="B10" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="23">
+        <v>2</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>76</v>
+      </c>
       <c r="J10" s="19"/>
       <c r="K10" s="24"/>
       <c r="L10" s="19"/>
@@ -2346,14 +2643,30 @@
       <c r="A11" s="24">
         <v>9</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
+      <c r="B11" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="23">
+        <v>2</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>74</v>
+      </c>
       <c r="J11" s="19"/>
       <c r="K11" s="24"/>
       <c r="L11" s="19"/>
@@ -2362,62 +2675,126 @@
       <c r="A12" s="24">
         <v>10</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
+      <c r="B12" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="23">
+        <v>2</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>78</v>
+      </c>
       <c r="J12" s="19"/>
       <c r="K12" s="24"/>
       <c r="L12" s="19"/>
     </row>
-    <row r="13" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
         <v>11</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
+      <c r="B13" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="23">
+        <v>2</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>85</v>
+      </c>
       <c r="J13" s="19"/>
       <c r="K13" s="24"/>
       <c r="L13" s="19"/>
     </row>
-    <row r="14" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
         <v>12</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="B14" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="23">
+        <v>2</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>89</v>
+      </c>
       <c r="J14" s="19"/>
       <c r="K14" s="24"/>
       <c r="L14" s="19"/>
     </row>
-    <row r="15" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
         <v>13</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+      <c r="B15" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="23">
+        <v>2</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>97</v>
+      </c>
       <c r="J15" s="19"/>
       <c r="K15" s="24"/>
       <c r="L15" s="19"/>
@@ -2426,78 +2803,158 @@
       <c r="A16" s="24">
         <v>14</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="B16" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="23">
+        <v>2</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>96</v>
+      </c>
       <c r="J16" s="19"/>
       <c r="K16" s="24"/>
       <c r="L16" s="19"/>
     </row>
-    <row r="17" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
         <v>15</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="B17" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="23">
+        <v>2</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>100</v>
+      </c>
       <c r="J17" s="19"/>
       <c r="K17" s="24"/>
       <c r="L17" s="19"/>
     </row>
-    <row r="18" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <v>16</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
+      <c r="B18" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="23">
+        <v>2</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="J18" s="19"/>
       <c r="K18" s="24"/>
       <c r="L18" s="19"/>
     </row>
-    <row r="19" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24">
         <v>17</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
+      <c r="B19" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="23">
+        <v>2</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="J19" s="19"/>
       <c r="K19" s="24"/>
       <c r="L19" s="19"/>
     </row>
-    <row r="20" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
         <v>18</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
+      <c r="B20" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="23">
+        <v>2</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>106</v>
+      </c>
       <c r="J20" s="19"/>
       <c r="K20" s="24"/>
       <c r="L20" s="19"/>
@@ -2506,14 +2963,30 @@
       <c r="A21" s="24">
         <v>19</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
+      <c r="B21" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="23">
+        <v>2</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>115</v>
+      </c>
       <c r="J21" s="19"/>
       <c r="K21" s="24"/>
       <c r="L21" s="19"/>
@@ -2806,13 +3279,13 @@
       <c r="K39" s="24"/>
       <c r="L39" s="19"/>
     </row>
-    <row r="40" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24">
         <v>38</v>
       </c>
       <c r="B40" s="24"/>
       <c r="C40" s="19"/>
-      <c r="D40" s="29"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="23"/>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
@@ -2822,13 +3295,13 @@
       <c r="K40" s="24"/>
       <c r="L40" s="19"/>
     </row>
-    <row r="41" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="24">
         <v>39</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
+      <c r="D41" s="29"/>
       <c r="E41" s="23"/>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
@@ -3062,13 +3535,13 @@
       <c r="K55" s="24"/>
       <c r="L55" s="19"/>
     </row>
-    <row r="56" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24">
         <v>54</v>
       </c>
       <c r="B56" s="24"/>
       <c r="C56" s="19"/>
-      <c r="D56" s="29"/>
+      <c r="D56" s="19"/>
       <c r="E56" s="23"/>
       <c r="F56" s="19"/>
       <c r="G56" s="19"/>
@@ -3078,13 +3551,13 @@
       <c r="K56" s="24"/>
       <c r="L56" s="19"/>
     </row>
-    <row r="57" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="24">
         <v>55</v>
       </c>
       <c r="B57" s="24"/>
       <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
+      <c r="D57" s="29"/>
       <c r="E57" s="23"/>
       <c r="F57" s="19"/>
       <c r="G57" s="19"/>
@@ -3324,7 +3797,7 @@
       </c>
       <c r="B72" s="24"/>
       <c r="C72" s="19"/>
-      <c r="D72" s="31"/>
+      <c r="D72" s="19"/>
       <c r="E72" s="23"/>
       <c r="F72" s="19"/>
       <c r="G72" s="19"/>
@@ -3340,7 +3813,7 @@
       </c>
       <c r="B73" s="24"/>
       <c r="C73" s="19"/>
-      <c r="D73" s="19"/>
+      <c r="D73" s="31"/>
       <c r="E73" s="23"/>
       <c r="F73" s="19"/>
       <c r="G73" s="19"/>
@@ -3590,302 +4063,331 @@
       <c r="K88" s="24"/>
       <c r="L88" s="19"/>
     </row>
+    <row r="89" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="24">
+        <v>87</v>
+      </c>
+      <c r="B89" s="24"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="19"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="19"/>
+      <c r="I89" s="19"/>
+      <c r="J89" s="19"/>
+      <c r="K89" s="24"/>
+      <c r="L89" s="19"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:L88"/>
+  <autoFilter ref="A2:L89"/>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="K1:K19">
-    <cfRule type="containsText" dxfId="82" priority="81" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K1:K17 K19:K20">
+    <cfRule type="containsText" dxfId="88" priority="84" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K19">
-    <cfRule type="containsText" dxfId="81" priority="79" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K3:K17 K19:K20">
+    <cfRule type="containsText" dxfId="87" priority="82" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="80" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="86" priority="83" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="79" priority="75" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="78" priority="73" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="74" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="76" priority="72" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="85" priority="78" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="75" priority="70" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="84" priority="76" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="71" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="83" priority="77" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22:K28">
-    <cfRule type="containsText" dxfId="73" priority="69" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K22">
+    <cfRule type="containsText" dxfId="82" priority="75" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K22)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22:K28">
-    <cfRule type="containsText" dxfId="72" priority="67" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K22">
+    <cfRule type="containsText" dxfId="81" priority="73" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="68" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="80" priority="74" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K22)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
-    <cfRule type="containsText" dxfId="70" priority="66" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
-    <cfRule type="containsText" dxfId="69" priority="64" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="65" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K29)))</formula>
+  <conditionalFormatting sqref="K23:K29">
+    <cfRule type="containsText" dxfId="79" priority="72" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23:K29">
+    <cfRule type="containsText" dxfId="78" priority="70" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="71" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="67" priority="63" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="76" priority="69" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="66" priority="61" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="75" priority="67" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="62" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="74" priority="68" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="64" priority="60" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="73" priority="66" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="63" priority="58" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="72" priority="64" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="59" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="71" priority="65" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32:K44">
-    <cfRule type="containsText" dxfId="61" priority="57" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K32">
+    <cfRule type="containsText" dxfId="70" priority="63" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32:K44">
-    <cfRule type="containsText" dxfId="60" priority="55" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K32">
+    <cfRule type="containsText" dxfId="69" priority="61" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="56" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="68" priority="62" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K45">
-    <cfRule type="containsText" dxfId="58" priority="54" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45">
-    <cfRule type="containsText" dxfId="57" priority="52" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="53" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K45)))</formula>
+  <conditionalFormatting sqref="K33:K45">
+    <cfRule type="containsText" dxfId="67" priority="60" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33:K45">
+    <cfRule type="containsText" dxfId="66" priority="58" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="59" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46">
-    <cfRule type="containsText" dxfId="55" priority="51" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="64" priority="57" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46">
-    <cfRule type="containsText" dxfId="54" priority="49" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="63" priority="55" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="50" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="62" priority="56" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="containsText" dxfId="52" priority="48" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="containsText" dxfId="51" priority="46" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="60" priority="52" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="47" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="59" priority="53" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K48:K54">
-    <cfRule type="containsText" dxfId="49" priority="45" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K48">
+    <cfRule type="containsText" dxfId="58" priority="51" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K48:K54">
-    <cfRule type="containsText" dxfId="48" priority="43" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K48">
+    <cfRule type="containsText" dxfId="57" priority="49" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="44" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="56" priority="50" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K55:K60">
-    <cfRule type="containsText" dxfId="46" priority="30" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K55:K60">
-    <cfRule type="containsText" dxfId="45" priority="28" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="29" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K61">
-    <cfRule type="containsText" dxfId="43" priority="27" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K61)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K61">
-    <cfRule type="containsText" dxfId="42" priority="25" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="26" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K61)))</formula>
+  <conditionalFormatting sqref="K49:K55">
+    <cfRule type="containsText" dxfId="55" priority="48" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K55">
+    <cfRule type="containsText" dxfId="54" priority="46" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="47" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56:K61">
+    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56:K61">
+    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="32" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="containsText" dxfId="40" priority="24" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="containsText" dxfId="39" priority="22" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="23" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="47" priority="29" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63">
-    <cfRule type="containsText" dxfId="37" priority="21" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63">
-    <cfRule type="containsText" dxfId="36" priority="19" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="20" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K64:K70">
-    <cfRule type="containsText" dxfId="34" priority="18" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K64">
+    <cfRule type="containsText" dxfId="43" priority="24" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K64)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K64:K70">
-    <cfRule type="containsText" dxfId="33" priority="16" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K64">
+    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="17" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K64)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K71:K78">
-    <cfRule type="containsText" dxfId="31" priority="15" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K71)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71:K78">
-    <cfRule type="containsText" dxfId="30" priority="13" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K71)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="14" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K71)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K79">
-    <cfRule type="containsText" dxfId="28" priority="12" operator="containsText" text="Blocked">
-      <formula>NOT(ISERROR(SEARCH("Blocked",K79)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K79">
-    <cfRule type="containsText" dxfId="27" priority="10" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",K79)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="11" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",K79)))</formula>
+  <conditionalFormatting sqref="K65:K71">
+    <cfRule type="containsText" dxfId="40" priority="21" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65:K71">
+    <cfRule type="containsText" dxfId="39" priority="19" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="20" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72:K79">
+    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72:K79">
+    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K72)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="17" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K80">
-    <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K80">
-    <cfRule type="containsText" dxfId="24" priority="7" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K80)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="8" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K81">
-    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="31" priority="12" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K81">
-    <cfRule type="containsText" dxfId="21" priority="4" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K81)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K82:K88">
-    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="K82">
+    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K82)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K82:K88">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="K82">
+    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K82)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K82)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K83:K89">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K83:K89">
+    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K83)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K88">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K89">
       <formula1>"Passed, Failed, Blocked"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E88">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E89">
       <formula1>"1, 2, 3"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4048,77 +4550,77 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="L1">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="17" priority="12" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="16" priority="10" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",L7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",L7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",L7)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>